<commit_message>
Improved demo9, added std::setlocale to get currencySumbol, check utf_8 changed styles
</commit_message>
<xml_diff>
--- a/Tests/NumberType.xlsx
+++ b/Tests/NumberType.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Dev\OpenXLSX\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FAA3856-9B48-4AA2-BF30-B47400B2D781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72A88D8-6206-4481-AB66-372C58742787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="5265" windowWidth="22080" windowHeight="11925" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24360" yWindow="5865" windowWidth="22080" windowHeight="11925" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>string</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -33,9 +37,9 @@
   <numFmts count="5">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="164" formatCode="[$¥-804]#,##0.00"/>
-    <numFmt numFmtId="166" formatCode="[$₿]\ #,##0.000000" x16r2:formatCode16="[$₿-x-xbt2]\ #,##0.000000"/>
-    <numFmt numFmtId="167" formatCode="[$-10464]dddd\,\ mmmm\ d\,\ yyyy;@"/>
-    <numFmt numFmtId="168" formatCode="m/d/yy\ h:mm;@"/>
+    <numFmt numFmtId="165" formatCode="[$₿]\ #,##0.000000" x16r2:formatCode16="[$₿-x-xbt2]\ #,##0.000000"/>
+    <numFmt numFmtId="166" formatCode="[$-10464]dddd\,\ mmmm\ d\,\ yyyy;@"/>
+    <numFmt numFmtId="167" formatCode="m/d/yy\ h:mm;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -71,10 +75,10 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -355,10 +359,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -406,6 +410,11 @@
         <v>36464</v>
       </c>
     </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fixed some compiler warnings start on Font class, uses raw pointer for XMLNode TODO use unique pointer
</commit_message>
<xml_diff>
--- a/Tests/NumberType.xlsx
+++ b/Tests/NumberType.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Dev\OpenXLSX\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72A88D8-6206-4481-AB66-372C58742787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF18767D-1288-492D-BEFA-91AA7EC2EFD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24360" yWindow="5865" windowWidth="22080" windowHeight="11925" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,13 +41,19 @@
     <numFmt numFmtId="166" formatCode="[$-10464]dddd\,\ mmmm\ d\,\ yyyy;@"/>
     <numFmt numFmtId="167" formatCode="m/d/yy\ h:mm;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -70,7 +76,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -79,6 +85,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,8 +417,8 @@
         <v>36464</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added get methods to fonts         int         underline()const;         bool        strikethrough() const;         bool        bold() const;         bool        italic() const;
note:
   alignment is in cellXfs, revise to cache the node to lookup
   applyXXX attributes, alignment and stuff we missed.
   lazy cache may be best
</commit_message>
<xml_diff>
--- a/Tests/NumberType.xlsx
+++ b/Tests/NumberType.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Dev\OpenXLSX\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF18767D-1288-492D-BEFA-91AA7EC2EFD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA0BADB-300A-49DC-AF3D-BC6CE8CA2FAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,9 +26,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="2">
   <si>
     <t>string</t>
+  </si>
+  <si>
+    <t>hello world</t>
   </si>
 </sst>
 </file>
@@ -41,7 +45,7 @@
     <numFmt numFmtId="166" formatCode="[$-10464]dddd\,\ mmmm\ d\,\ yyyy;@"/>
     <numFmt numFmtId="167" formatCode="m/d/yy\ h:mm;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,6 +58,52 @@
       <color rgb="FFFF0000"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u val="double"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -76,7 +126,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -86,6 +136,12 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -368,7 +424,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -426,4 +482,53 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3611CB75-0751-4E64-B6F7-710FB512D7D5}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>